<commit_message>
Minor mods to the charts
</commit_message>
<xml_diff>
--- a/examples/HexapodTiming.xlsx
+++ b/examples/HexapodTiming.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\AnimatLabSDK\3rdParty\openFrameworksArduino\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6960" activeTab="4"/>
   </bookViews>
@@ -18,7 +13,7 @@
     <sheet name="6 Legs" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="19">
   <si>
     <t>Avg_2Legs</t>
   </si>
@@ -79,6 +74,12 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>Milliseconds</t>
+  </si>
+  <si>
+    <t>Update Rate</t>
   </si>
 </sst>
 </file>
@@ -198,26 +199,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -309,7 +290,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$F$11:$F$13</c:f>
+                <c:f>Sheet4!$H$11:$H$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -327,7 +308,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$F$11:$F$13</c:f>
+                <c:f>Sheet4!$H$11:$H$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -403,11 +384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="221114896"/>
-        <c:axId val="252923608"/>
+        <c:axId val="177296512"/>
+        <c:axId val="177298432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="221114896"/>
+        <c:axId val="177296512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -463,26 +444,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -521,12 +482,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252923608"/>
+        <c:crossAx val="177298432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252923608"/>
+        <c:axId val="177298432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,26 +542,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -639,7 +580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221114896"/>
+        <c:crossAx val="177296512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -737,26 +678,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -848,7 +769,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$G$11:$G$13</c:f>
+                <c:f>Sheet4!$I$11:$I$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -866,7 +787,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$G$11:$G$13</c:f>
+                <c:f>Sheet4!$I$11:$I$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -916,7 +837,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$C$11:$C$13</c:f>
+              <c:f>Sheet4!$D$11:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -942,11 +863,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="454470888"/>
-        <c:axId val="454471280"/>
+        <c:axId val="81342848"/>
+        <c:axId val="81344768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="454470888"/>
+        <c:axId val="81342848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -1002,26 +923,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1060,12 +961,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454471280"/>
+        <c:crossAx val="81344768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="454471280"/>
+        <c:axId val="81344768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,26 +1021,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1178,7 +1059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454470888"/>
+        <c:crossAx val="81342848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1276,26 +1157,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1387,7 +1248,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$I$3:$I$5</c:f>
+                <c:f>Sheet4!$K$3:$K$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1405,7 +1266,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$I$3:$I$5</c:f>
+                <c:f>Sheet4!$K$3:$K$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1481,11 +1342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="452411176"/>
-        <c:axId val="454470496"/>
+        <c:axId val="81376384"/>
+        <c:axId val="81378304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="452411176"/>
+        <c:axId val="81376384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -1541,26 +1402,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1599,12 +1440,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="454470496"/>
+        <c:crossAx val="81378304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="454470496"/>
+        <c:axId val="81378304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,26 +1500,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1717,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452411176"/>
+        <c:crossAx val="81376384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1815,26 +1636,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1940,7 +1741,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$K$3:$K$5</c:f>
+                <c:f>Sheet4!$M$3:$M$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1958,7 +1759,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$K$3:$K$5</c:f>
+                <c:f>Sheet4!$M$3:$M$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -2008,7 +1809,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$D$3:$D$5</c:f>
+              <c:f>Sheet4!$E$3:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2034,11 +1835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453375760"/>
-        <c:axId val="252704216"/>
+        <c:axId val="176297088"/>
+        <c:axId val="176299008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="453375760"/>
+        <c:axId val="176297088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -2094,26 +1895,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2152,12 +1933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252704216"/>
+        <c:crossAx val="176299008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252704216"/>
+        <c:axId val="176299008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2212,26 +1993,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2270,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453375760"/>
+        <c:crossAx val="176297088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4553,7 +4314,7 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -4583,7 +4344,7 @@
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
@@ -4607,13 +4368,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -4639,13 +4400,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -4927,7 +4688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6707,7 +6468,7 @@
   <dimension ref="A1:N106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7305,66 +7066,88 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <f>1/(S2/1000)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -7373,51 +7156,66 @@
         <v>24.830322222222222</v>
       </c>
       <c r="C3">
+        <f>1/(B3/1000)</f>
+        <v>40.273339630890369</v>
+      </c>
+      <c r="D3">
         <f>'2 Legs'!B47</f>
         <v>25.502873684210527</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>'2 Legs'!C47</f>
         <v>20.108170833333329</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <f>1/(E3/1000)</f>
+        <v>49.731027664749064</v>
+      </c>
+      <c r="G3">
         <f>'2 Legs'!D47</f>
         <v>24.525636842105264</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <f>'2 Legs'!E47</f>
         <v>28.287187499999998</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <f>'2 Legs'!F47</f>
         <v>30.557743749999997</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <f>'2 Legs'!A48</f>
         <v>7.2621798516205756</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <f>'2 Legs'!B48</f>
         <v>6.8678114948107547</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <f>'2 Legs'!C48</f>
         <v>5.1651690461590327</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <f>'2 Legs'!D48</f>
         <v>5.9351821430136447</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <f>'2 Legs'!E48</f>
         <v>3.3418504710854418</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <f>'2 Legs'!F48</f>
         <v>4.9767461370318262</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T31" si="0">1/(S3/1000)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -7426,51 +7224,66 @@
         <v>57.438499999999998</v>
       </c>
       <c r="C4">
+        <f t="shared" ref="C4:C6" si="1">1/(B4/1000)</f>
+        <v>17.409925398469667</v>
+      </c>
+      <c r="D4">
         <f>'4 Legs'!B27</f>
         <v>44.729355555555557</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>'4 Legs'!C27</f>
         <v>46.006340000000002</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <f t="shared" ref="F4:F6" si="2">1/(E4/1000)</f>
+        <v>21.736134628401217</v>
+      </c>
+      <c r="G4">
         <f>'4 Legs'!D27</f>
         <v>35.965741666666666</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <f>'4 Legs'!E27</f>
         <v>31.936300000000003</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <f>'4 Legs'!F27</f>
         <v>39.524463636363635</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f>'4 Legs'!A28</f>
         <v>20.375406965961975</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <f>'4 Legs'!B28</f>
         <v>19.782756819631871</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <f>'4 Legs'!C28</f>
         <v>15.480777276106005</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <f>'4 Legs'!D28</f>
         <v>6.1245391968781879</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <f>'4 Legs'!E28</f>
         <v>5.827988476309808</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <f>'4 Legs'!F28</f>
         <v>11.813968094842254</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18</v>
       </c>
@@ -7479,106 +7292,161 @@
         <v>54.420555555555552</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>18.37540961850608</v>
+      </c>
+      <c r="D5">
         <f>'6 Legs'!B27</f>
         <v>81.598579999999998</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>'6 Legs'!C27</f>
         <v>56.634774999999998</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>17.656996077056895</v>
+      </c>
+      <c r="G5">
         <f>'6 Legs'!D27</f>
         <v>42.034720000000007</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <f>'6 Legs'!E27</f>
         <v>39.263250000000006</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <f>'6 Legs'!F27</f>
         <v>43.037750000000003</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f>'6 Legs'!A28</f>
         <v>23.208055188524114</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <f>'6 Legs'!B28</f>
         <v>52.051146314270532</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <f>'6 Legs'!C28</f>
         <v>16.340187807194109</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <f>'6 Legs'!D28</f>
         <v>14.131124917627735</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <f>'6 Legs'!E28</f>
         <v>7.0074131942179259</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <f>'6 Legs'!F28</f>
         <v>7.0128111072878383</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <v>20</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <f>2.46559*A6+15.973</f>
-        <v>75.14716</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2">
+        <v>85.009520000000009</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>11.76338838285406</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
         <f>3.0439*A6+4.3898</f>
-        <v>77.443399999999983</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <f>1/(B6/1000)</f>
-        <v>13.307222787927047</v>
-      </c>
-      <c r="D7">
-        <f>1/(D6/1000)</f>
-        <v>12.912656210858515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89.618999999999986</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>11.158348118144591</v>
+      </c>
+      <c r="S6">
+        <v>25</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <v>30</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>35</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>40</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <v>45</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>22.222222222222221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -7587,27 +7455,42 @@
         <v>37.413691666666665</v>
       </c>
       <c r="C11">
+        <f>1/(B11/1000)</f>
+        <v>26.728183064889571</v>
+      </c>
+      <c r="D11">
         <f>'2 Legs'!B79</f>
         <v>27.298193749999999</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <f>1/(D11/1000)</f>
+        <v>36.632460343644532</v>
+      </c>
+      <c r="F11">
         <f>'2 Legs'!C79</f>
         <v>34.119785714285705</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <f>'2 Legs'!A80</f>
         <v>13.52946991641201</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <f>'2 Legs'!B80</f>
         <v>7.4352328918189174</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <f>'2 Legs'!C80</f>
         <v>5.3935574089910228</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>50</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -7616,27 +7499,42 @@
         <v>62.189566666666657</v>
       </c>
       <c r="C12">
+        <f t="shared" ref="C12:C14" si="3">1/(B12/1000)</f>
+        <v>16.079867630529669</v>
+      </c>
+      <c r="D12">
         <f>'4 Legs'!B62</f>
         <v>48.12177777777778</v>
       </c>
-      <c r="D12">
+      <c r="E12">
+        <f t="shared" ref="E12:E14" si="4">1/(D12/1000)</f>
+        <v>20.780612150654822</v>
+      </c>
+      <c r="F12">
         <f>'4 Legs'!C62</f>
         <v>53.66451428571429</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <f>'4 Legs'!A63</f>
         <v>36.877164760307828</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <f>'4 Legs'!B63</f>
         <v>16.959798928693946</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <f>'4 Legs'!C63</f>
         <v>14.61194696076061</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>55</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>18.181818181818183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -7645,27 +7543,42 @@
         <v>89.826799999999992</v>
       </c>
       <c r="C13">
+        <f t="shared" si="3"/>
+        <v>11.132535056352893</v>
+      </c>
+      <c r="D13">
         <f>'6 Legs'!B105</f>
         <v>56.720500000000001</v>
       </c>
-      <c r="D13">
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>17.630310029001858</v>
+      </c>
+      <c r="F13">
         <f>'6 Legs'!C105</f>
         <v>55.260399999999997</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <f>'6 Legs'!A106</f>
         <v>23.871419449626362</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <f>'6 Legs'!B106</f>
         <v>19.204764256689014</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <f>'6 Legs'!C106</f>
         <v>13.707499264271384</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <v>60</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>24</v>
       </c>
@@ -7673,22 +7586,177 @@
         <f>4.3678*A14+10.73</f>
         <v>115.55720000000001</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>8.653723004711086</v>
+      </c>
+      <c r="D14" s="2">
         <f>2.4519*A14+14.625</f>
         <v>73.470600000000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <f>1/(B14/1000)</f>
-        <v>8.653723004711086</v>
-      </c>
-      <c r="C15">
-        <f>1/(C14/1000)</f>
+      <c r="E14">
+        <f t="shared" si="4"/>
         <v>13.61088653148334</v>
+      </c>
+      <c r="S14">
+        <v>65</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>15.384615384615383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <v>70</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>14.285714285714285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <v>75</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <v>80</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="18" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S18">
+        <v>85</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>11.76470588235294</v>
+      </c>
+    </row>
+    <row r="19" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S19">
+        <v>90</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>11.111111111111111</v>
+      </c>
+    </row>
+    <row r="20" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S20">
+        <v>95</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="0"/>
+        <v>10.526315789473685</v>
+      </c>
+    </row>
+    <row r="21" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <v>100</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <v>105</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>9.5238095238095237</v>
+      </c>
+    </row>
+    <row r="23" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>110</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="24" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>115</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>8.695652173913043</v>
+      </c>
+    </row>
+    <row r="25" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>120</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="26" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>125</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>130</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076916</v>
+      </c>
+    </row>
+    <row r="28" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>135</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>7.4074074074074066</v>
+      </c>
+    </row>
+    <row r="29" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S29">
+        <v>140</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571423</v>
+      </c>
+    </row>
+    <row r="30" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>145</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>6.8965517241379315</v>
+      </c>
+    </row>
+    <row r="31" spans="19:20" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>150</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code to set the return delay time.
</commit_message>
<xml_diff>
--- a/examples/HexapodTiming.xlsx
+++ b/examples/HexapodTiming.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\AnimatLabSDK\3rdParty\openFrameworksArduino\examples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6960" activeTab="4"/>
   </bookViews>
@@ -11,9 +16,9 @@
     <sheet name="2 Legs" sheetId="2" r:id="rId2"/>
     <sheet name="4 Legs" sheetId="3" r:id="rId3"/>
     <sheet name="6 Legs" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Analysis" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -199,6 +204,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -290,7 +315,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$H$11:$H$13</c:f>
+                <c:f>Analysis!$H$11:$H$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -308,7 +333,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$H$11:$H$13</c:f>
+                <c:f>Analysis!$H$11:$H$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -340,7 +365,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$11:$A$13</c:f>
+              <c:f>Analysis!$A$11:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -358,7 +383,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$B$11:$B$13</c:f>
+              <c:f>Analysis!$B$11:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -384,11 +409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="167924864"/>
-        <c:axId val="167926784"/>
+        <c:axId val="216139864"/>
+        <c:axId val="216763200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="167924864"/>
+        <c:axId val="216139864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -444,6 +469,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -482,12 +527,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167926784"/>
+        <c:crossAx val="216763200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="167926784"/>
+        <c:axId val="216763200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,6 +587,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -580,7 +645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="167924864"/>
+        <c:crossAx val="216139864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -678,6 +743,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -769,7 +854,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$I$11:$I$13</c:f>
+                <c:f>Analysis!$I$11:$I$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -787,7 +872,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$I$11:$I$13</c:f>
+                <c:f>Analysis!$I$11:$I$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -819,7 +904,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$11:$A$13</c:f>
+              <c:f>Analysis!$A$11:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -837,7 +922,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$D$11:$D$13</c:f>
+              <c:f>Analysis!$D$11:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -863,11 +948,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169558400"/>
-        <c:axId val="169560320"/>
+        <c:axId val="216564208"/>
+        <c:axId val="216585600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169558400"/>
+        <c:axId val="216564208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -923,6 +1008,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -961,12 +1066,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169560320"/>
+        <c:crossAx val="216585600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169560320"/>
+        <c:axId val="216585600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,6 +1126,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1059,7 +1184,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169558400"/>
+        <c:crossAx val="216564208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1157,6 +1282,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1248,7 +1393,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$K$3:$K$5</c:f>
+                <c:f>Analysis!$K$3:$K$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1266,7 +1411,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$K$3:$K$5</c:f>
+                <c:f>Analysis!$K$3:$K$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1298,7 +1443,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$3:$A$5</c:f>
+              <c:f>Analysis!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1316,7 +1461,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$B$3:$B$5</c:f>
+              <c:f>Analysis!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1342,11 +1487,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169586048"/>
-        <c:axId val="169592320"/>
+        <c:axId val="216588256"/>
+        <c:axId val="216739256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169586048"/>
+        <c:axId val="216588256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -1402,6 +1547,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1440,12 +1605,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169592320"/>
+        <c:crossAx val="216739256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169592320"/>
+        <c:axId val="216739256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,6 +1665,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1538,7 +1723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169586048"/>
+        <c:crossAx val="216588256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1636,6 +1821,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1741,7 +1946,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet4!$M$3:$M$5</c:f>
+                <c:f>Analysis!$M$3:$M$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1759,7 +1964,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet4!$M$3:$M$5</c:f>
+                <c:f>Analysis!$M$3:$M$5</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1791,7 +1996,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$3:$A$5</c:f>
+              <c:f>Analysis!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1809,7 +2014,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$E$3:$E$5</c:f>
+              <c:f>Analysis!$E$3:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1835,11 +2040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169661568"/>
-        <c:axId val="169663488"/>
+        <c:axId val="216738336"/>
+        <c:axId val="214667968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169661568"/>
+        <c:axId val="216738336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -1895,6 +2100,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1933,12 +2158,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169663488"/>
+        <c:crossAx val="214667968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169663488"/>
+        <c:axId val="214667968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,6 +2218,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2031,7 +2276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169661568"/>
+        <c:crossAx val="216738336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2141,7 +2386,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$E$2</c:f>
+              <c:f>Analysis!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2161,7 +2406,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$3:$A$5</c:f>
+              <c:f>Analysis!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2179,7 +2424,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$F$3:$F$5</c:f>
+              <c:f>Analysis!$F$3:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2205,11 +2450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169725952"/>
-        <c:axId val="169727872"/>
+        <c:axId val="216416792"/>
+        <c:axId val="216417184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169725952"/>
+        <c:axId val="216416792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5"/>
@@ -2303,12 +2548,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169727872"/>
+        <c:crossAx val="216417184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169727872"/>
+        <c:axId val="216417184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,7 +2646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169725952"/>
+        <c:crossAx val="216416792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2475,7 +2720,7 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$11:$A$13</c:f>
+              <c:f>Analysis!$A$11:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2493,7 +2738,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$C$11:$C$13</c:f>
+              <c:f>Analysis!$C$11:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2516,7 +2761,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$D$10</c:f>
+              <c:f>Analysis!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2527,7 +2772,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet4!$A$11:$A$13</c:f>
+              <c:f>Analysis!$A$11:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2545,7 +2790,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet4!$E$11:$E$13</c:f>
+              <c:f>Analysis!$E$11:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2571,11 +2816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="169737216"/>
-        <c:axId val="169743104"/>
+        <c:axId val="216418360"/>
+        <c:axId val="216418752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="169737216"/>
+        <c:axId val="216418360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2585,12 +2830,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169743104"/>
+        <c:crossAx val="216418752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="169743104"/>
+        <c:axId val="216418752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2601,7 +2846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169737216"/>
+        <c:crossAx val="216418360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5293,7 +5538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7674,7 +7919,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="A11:A13 C11:C13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8185,23 +8430,23 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <f>4.3678*A14+10.73</f>
-        <v>115.55720000000001</v>
+        <v>133.0284</v>
       </c>
       <c r="C14">
         <f t="shared" si="3"/>
-        <v>8.653723004711086</v>
+        <v>7.5171918176870509</v>
       </c>
       <c r="D14" s="2">
         <f>2.4519*A14+14.625</f>
-        <v>73.470600000000005</v>
+        <v>83.278199999999998</v>
       </c>
       <c r="E14">
         <f t="shared" si="4"/>
-        <v>13.61088653148334</v>
+        <v>12.007944456052124</v>
       </c>
       <c r="S14">
         <v>65</v>

</xml_diff>